<commit_message>
Updated batch file processing
</commit_message>
<xml_diff>
--- a/test_run/target_enrollment.xlsx
+++ b/test_run/target_enrollment.xlsx
@@ -467,7 +467,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -490,7 +490,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -513,7 +513,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -536,7 +536,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -559,7 +559,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>

</xml_diff>